<commit_message>
Date fixing and generate_json set to false by default
</commit_message>
<xml_diff>
--- a/Crawler/spiders/BNA_advanced_search.xlsx
+++ b/Crawler/spiders/BNA_advanced_search.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\KOSTA\Documentos\Durham\VictorialElectionViolenceCrawl\Crawler\spiders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586E590B-027B-41F3-B6D8-3536A226D7DD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086F0624-C8ED-4992-A862-68B08E80C6D4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{66E8729E-A97F-4DF0-A7A0-088B1D4505B9}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="1412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="1416">
   <si>
     <t>Search some words</t>
   </si>
@@ -4265,15 +4265,24 @@
   </si>
   <si>
     <t>Article,Illustrated</t>
+  </si>
+  <si>
+    <t>1980-01-01</t>
+  </si>
+  <si>
+    <t>1964-01-01</t>
+  </si>
+  <si>
+    <t>2016-01-01</t>
+  </si>
+  <si>
+    <t>2018-01-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4319,27 +4328,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4368,12 +4377,12 @@
     <tableColumn id="5" xr3:uid="{3D8B7C87-A6C5-4A08-AC62-0207662F9ACE}" name="Exact search" dataDxfId="5"/>
     <tableColumn id="6" xr3:uid="{F8B91DAD-253E-400C-8A3C-C34BC799C62F}" name="Publication place"/>
     <tableColumn id="16" xr3:uid="{7350EE25-8ED3-45ED-8BE9-C1A261A68C6D}" name="Newspaper title"/>
-    <tableColumn id="7" xr3:uid="{0A8E4D80-E09E-4BC5-88C0-F9A6AD4009F9}" name="From date" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{ABB5D4A5-62F1-4B65-BDF9-1CCADC7812B1}" name="To date" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{6CB285D8-4622-4089-89C7-F93CFCF7EF2A}" name="From date added" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{01CEA437-C27B-43C8-9696-4BE712ADCDA1}" name="To date added" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{0A8E4D80-E09E-4BC5-88C0-F9A6AD4009F9}" name="From date" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{ABB5D4A5-62F1-4B65-BDF9-1CCADC7812B1}" name="To date" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{6CB285D8-4622-4089-89C7-F93CFCF7EF2A}" name="From date added" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{01CEA437-C27B-43C8-9696-4BE712ADCDA1}" name="To date added" dataDxfId="0"/>
     <tableColumn id="11" xr3:uid="{09AF702E-9894-4802-93E1-78C118A4179C}" name="Article Type"/>
-    <tableColumn id="12" xr3:uid="{E41FEA5A-0C84-4887-9842-987FEAEA16C8}" name="Front page articles only" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{E41FEA5A-0C84-4887-9842-987FEAEA16C8}" name="Front page articles only" dataDxfId="4"/>
     <tableColumn id="13" xr3:uid="{C218A81E-A465-4F8C-8633-F3FF131C5161}" name="Tags"/>
     <tableColumn id="14" xr3:uid="{1F81B7FC-677C-429A-BC4E-D0E9B2CDAA8A}" name="Sort results by"/>
   </tableColumns>
@@ -4680,8 +4689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA51FF3A-7312-4144-AFEF-8EFFA538FD87}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4693,10 +4702,10 @@
     <col min="5" max="5" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.08984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.08984375" customWidth="1"/>
-    <col min="8" max="8" width="11.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.90625" style="3"/>
-    <col min="10" max="10" width="17.1796875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="14.90625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="11.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.90625" style="4"/>
+    <col min="10" max="10" width="17.1796875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="14.90625" style="4" customWidth="1"/>
     <col min="12" max="12" width="12.6328125" customWidth="1"/>
     <col min="13" max="13" width="22.26953125" customWidth="1"/>
     <col min="14" max="14" width="32.81640625" customWidth="1"/>
@@ -4726,16 +4735,16 @@
       <c r="G1" t="s">
         <v>978</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="L1" t="s">
@@ -4767,17 +4776,17 @@
       <c r="G2" t="s">
         <v>638</v>
       </c>
-      <c r="H2" s="3">
-        <v>23377</v>
-      </c>
-      <c r="I2" s="3">
-        <v>29586</v>
-      </c>
-      <c r="J2" s="3">
-        <v>42656</v>
-      </c>
-      <c r="K2" s="3">
-        <v>43294</v>
+      <c r="H2" s="4" t="s">
+        <v>1413</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>1412</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>1414</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>1415</v>
       </c>
       <c r="L2" t="s">
         <v>1411</v>
@@ -4792,7 +4801,7 @@
     <row r="3" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="4"/>
+      <c r="N3" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Candidate document article_title bug fixed. Advanced search saved into the database
</commit_message>
<xml_diff>
--- a/Crawler/spiders/BNA_advanced_search.xlsx
+++ b/Crawler/spiders/BNA_advanced_search.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\KOSTA\Documentos\Durham\VictorialElectionViolenceCrawl\Crawler\spiders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086F0624-C8ED-4992-A862-68B08E80C6D4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD9D004-CC24-4251-BD76-991AD63173CA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{66E8729E-A97F-4DF0-A7A0-088B1D4505B9}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="1416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="1416">
   <si>
     <t>Search some words</t>
   </si>
@@ -4336,7 +4336,7 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -4348,7 +4348,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4377,12 +4377,12 @@
     <tableColumn id="5" xr3:uid="{3D8B7C87-A6C5-4A08-AC62-0207662F9ACE}" name="Exact search" dataDxfId="5"/>
     <tableColumn id="6" xr3:uid="{F8B91DAD-253E-400C-8A3C-C34BC799C62F}" name="Publication place"/>
     <tableColumn id="16" xr3:uid="{7350EE25-8ED3-45ED-8BE9-C1A261A68C6D}" name="Newspaper title"/>
-    <tableColumn id="7" xr3:uid="{0A8E4D80-E09E-4BC5-88C0-F9A6AD4009F9}" name="From date" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{ABB5D4A5-62F1-4B65-BDF9-1CCADC7812B1}" name="To date" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{6CB285D8-4622-4089-89C7-F93CFCF7EF2A}" name="From date added" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{01CEA437-C27B-43C8-9696-4BE712ADCDA1}" name="To date added" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{0A8E4D80-E09E-4BC5-88C0-F9A6AD4009F9}" name="From date" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{ABB5D4A5-62F1-4B65-BDF9-1CCADC7812B1}" name="To date" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{6CB285D8-4622-4089-89C7-F93CFCF7EF2A}" name="From date added" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{01CEA437-C27B-43C8-9696-4BE712ADCDA1}" name="To date added" dataDxfId="1"/>
     <tableColumn id="11" xr3:uid="{09AF702E-9894-4802-93E1-78C118A4179C}" name="Article Type"/>
-    <tableColumn id="12" xr3:uid="{E41FEA5A-0C84-4887-9842-987FEAEA16C8}" name="Front page articles only" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{E41FEA5A-0C84-4887-9842-987FEAEA16C8}" name="Front page articles only" dataDxfId="0"/>
     <tableColumn id="13" xr3:uid="{C218A81E-A465-4F8C-8633-F3FF131C5161}" name="Tags"/>
     <tableColumn id="14" xr3:uid="{1F81B7FC-677C-429A-BC4E-D0E9B2CDAA8A}" name="Sort results by"/>
   </tableColumns>
@@ -4689,8 +4689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA51FF3A-7312-4144-AFEF-8EFFA538FD87}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4767,11 +4767,17 @@
       <c r="B2" t="s">
         <v>1409</v>
       </c>
+      <c r="C2" t="s">
+        <v>1408</v>
+      </c>
       <c r="D2" t="s">
         <v>1410</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1247</v>
       </c>
       <c r="G2" t="s">
         <v>638</v>

</xml_diff>

<commit_message>
Counting and split implemented
</commit_message>
<xml_diff>
--- a/Crawler/spiders/BNA_advanced_search.xlsx
+++ b/Crawler/spiders/BNA_advanced_search.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\KOSTA\Documentos\Durham\VictorialElectionViolenceCrawl\Crawler\spiders\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\KOSTA\Documentos\Durham\MSc\VictorialElectionViolenceCrawl\Crawler\spiders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD9D004-CC24-4251-BD76-991AD63173CA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40617A90-5F93-4C77-AF29-E60D47E449F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{66E8729E-A97F-4DF0-A7A0-088B1D4505B9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{66E8729E-A97F-4DF0-A7A0-088B1D4505B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="1416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="1411">
   <si>
     <t>Search some words</t>
   </si>
@@ -4255,28 +4255,13 @@
     <t>Date (most recent)</t>
   </si>
   <si>
-    <t>durham university</t>
-  </si>
-  <si>
-    <t>medical</t>
-  </si>
-  <si>
-    <t>newcastle</t>
-  </si>
-  <si>
-    <t>Article,Illustrated</t>
-  </si>
-  <si>
-    <t>1980-01-01</t>
-  </si>
-  <si>
-    <t>1964-01-01</t>
-  </si>
-  <si>
-    <t>2016-01-01</t>
-  </si>
-  <si>
-    <t>2018-01-01</t>
+    <t>mexico</t>
+  </si>
+  <si>
+    <t>1801-01-01</t>
+  </si>
+  <si>
+    <t>1801-02-02</t>
   </si>
 </sst>
 </file>
@@ -4367,8 +4352,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9B1CEB33-01FD-4B7D-B1DF-6803C7458733}" name="Tabla1" displayName="Tabla1" ref="A1:O2" totalsRowShown="0">
-  <autoFilter ref="A1:O2" xr:uid="{F04EF471-51A2-41F5-A449-A400148B94FE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9B1CEB33-01FD-4B7D-B1DF-6803C7458733}" name="Tabla1" displayName="Tabla1" ref="A1:O3" totalsRowShown="0">
+  <autoFilter ref="A1:O3" xr:uid="{F04EF471-51A2-41F5-A449-A400148B94FE}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{7DD74865-2221-4F23-B6C0-18D191CCA3C9}" name="Search all words"/>
     <tableColumn id="2" xr3:uid="{8E59F4EB-9F97-4A24-A2E3-DAD6E1BB128D}" name="Search some words"/>
@@ -4687,10 +4672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA51FF3A-7312-4144-AFEF-8EFFA538FD87}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4760,58 +4745,26 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1408</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" s="1"/>
+      <c r="H2" s="4" t="s">
         <v>1409</v>
       </c>
-      <c r="C2" t="s">
-        <v>1408</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="I2" s="4" t="s">
         <v>1410</v>
       </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1247</v>
-      </c>
-      <c r="G2" t="s">
-        <v>638</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>1413</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>1412</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>1414</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>1415</v>
-      </c>
       <c r="L2" t="s">
-        <v>1411</v>
-      </c>
-      <c r="M2" s="1">
-        <v>0</v>
-      </c>
-      <c r="O2" t="s">
-        <v>1406</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="3"/>
+        <v>1401</v>
+      </c>
+      <c r="M2" s="1"/>
+      <c r="N2" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M2 E1:E2" xr:uid="{CBAF3898-1E56-4BFE-AE4C-061993B6013C}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E2 M1:M2" xr:uid="{CBAF3898-1E56-4BFE-AE4C-061993B6013C}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -4828,7 +4781,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="2" id="{782709B5-0DC8-4A56-B6AE-83D33AED4CB5}">
+          <x14:cfRule type="iconSet" priority="3" id="{782709B5-0DC8-4A56-B6AE-83D33AED4CB5}">
             <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4847,7 +4800,7 @@
           <xm:sqref>E1:E2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{940BDCFA-B61F-4161-900D-26FC7C362201}">
+          <x14:cfRule type="iconSet" priority="5" id="{940BDCFA-B61F-4161-900D-26FC7C362201}">
             <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4869,6 +4822,12 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D22600C5-8745-46F6-B11C-6C5B25E3422C}">
+          <x14:formula1>
+            <xm:f>'Article types'!$A$1:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>L1</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00441275-8976-4C3C-A6FD-4AC89750ECF5}">
           <x14:formula1>
             <xm:f>Newspapers!$A:$A</xm:f>
@@ -4880,12 +4839,6 @@
             <xm:f>Places!$A$1:$A$421</xm:f>
           </x14:formula1>
           <xm:sqref>F2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D22600C5-8745-46F6-B11C-6C5B25E3422C}">
-          <x14:formula1>
-            <xm:f>'Article types'!$A$1:$A$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>L1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{318103E7-A071-46EE-A51F-7E8EB4D9F467}">
           <x14:formula1>

</xml_diff>